<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@c34eee24a3bfe40eddbc16270de27e01dd064f69 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-adi-documentreference.xlsx
+++ b/StructureDefinition-us-core-adi-documentreference.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="524">
   <si>
     <t>Property</t>
   </si>
@@ -475,6 +475,13 @@
   </si>
   <si>
     <t>US Core DocumentReference Authentication Time Extension"</t>
+  </si>
+  <si>
+    <t>When the information in the document was verified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
   </si>
   <si>
     <t>DocumentReference.modifierExtension</t>
@@ -3159,7 +3166,7 @@
         <v>147</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -3219,7 +3226,7 @@
         <v>81</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>143</v>
@@ -3248,14 +3255,14 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
@@ -3277,16 +3284,16 @@
         <v>137</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O11" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="P11" t="s" s="2">
         <v>21</v>
@@ -3335,7 +3342,7 @@
         <v>21</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>80</v>
@@ -3373,10 +3380,10 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -3399,19 +3406,19 @@
         <v>93</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="O12" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="P12" t="s" s="2">
         <v>21</v>
@@ -3460,7 +3467,7 @@
         <v>21</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>80</v>
@@ -3475,33 +3482,33 @@
         <v>104</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AO12" t="s" s="2">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="AP12" t="s" s="2">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AQ12" t="s" s="2">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -3524,13 +3531,13 @@
         <v>93</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -3581,7 +3588,7 @@
         <v>21</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>80</v>
@@ -3596,33 +3603,33 @@
         <v>104</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AN13" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AO13" t="s" s="2">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="AP13" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AQ13" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3648,13 +3655,13 @@
         <v>112</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
@@ -3680,11 +3687,11 @@
         <v>21</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Y14" s="2"/>
       <c r="Z14" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>21</v>
@@ -3702,7 +3709,7 @@
         <v>21</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>92</v>
@@ -3717,33 +3724,33 @@
         <v>104</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AN14" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AO14" t="s" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="AP14" t="s" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="AQ14" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3769,13 +3776,13 @@
         <v>112</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
@@ -3801,13 +3808,13 @@
         <v>21</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>21</v>
@@ -3825,7 +3832,7 @@
         <v>21</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>80</v>
@@ -3843,19 +3850,19 @@
         <v>21</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="AN15" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AO15" t="s" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="AP15" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="AQ15" t="s" s="2">
         <v>21</v>
@@ -3863,10 +3870,10 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3889,16 +3896,16 @@
         <v>93</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" t="s" s="2">
@@ -3924,13 +3931,13 @@
         <v>21</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>21</v>
@@ -3948,7 +3955,7 @@
         <v>21</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>80</v>
@@ -3963,37 +3970,37 @@
         <v>104</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AP16" t="s" s="2">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="AQ16" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
@@ -4012,16 +4019,16 @@
         <v>93</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" t="s" s="2">
@@ -4047,19 +4054,19 @@
         <v>21</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="Z17" t="s" s="2">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AB17" t="s" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="AC17" s="2"/>
       <c r="AD17" t="s" s="2">
@@ -4069,7 +4076,7 @@
         <v>141</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>80</v>
@@ -4087,36 +4094,36 @@
         <v>21</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AP17" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AQ17" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
@@ -4135,16 +4142,16 @@
         <v>93</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
@@ -4170,13 +4177,13 @@
         <v>21</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="Z18" t="s" s="2">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="AA18" t="s" s="2">
         <v>21</v>
@@ -4194,7 +4201,7 @@
         <v>21</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>80</v>
@@ -4212,30 +4219,30 @@
         <v>21</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AP18" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AQ18" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -4258,13 +4265,13 @@
         <v>93</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -4315,7 +4322,7 @@
         <v>21</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>80</v>
@@ -4330,37 +4337,37 @@
         <v>104</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AP19" t="s" s="2">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AQ19" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
@@ -4379,16 +4386,16 @@
         <v>93</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
@@ -4438,7 +4445,7 @@
         <v>21</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>80</v>
@@ -4453,19 +4460,19 @@
         <v>104</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AN20" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AP20" t="s" s="2">
         <v>21</v>
@@ -4476,10 +4483,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4502,16 +4509,16 @@
         <v>93</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -4561,7 +4568,7 @@
         <v>21</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>80</v>
@@ -4576,33 +4583,33 @@
         <v>104</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AP21" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="AQ21" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4625,16 +4632,16 @@
         <v>21</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
@@ -4684,7 +4691,7 @@
         <v>21</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>80</v>
@@ -4699,33 +4706,33 @@
         <v>104</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AP22" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AQ22" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4748,13 +4755,13 @@
         <v>21</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -4805,7 +4812,7 @@
         <v>21</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>80</v>
@@ -4826,7 +4833,7 @@
         <v>21</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>21</v>
@@ -4843,14 +4850,14 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4872,13 +4879,13 @@
         <v>137</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -4919,7 +4926,7 @@
         <v>140</v>
       </c>
       <c r="AC24" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AD24" t="s" s="2">
         <v>21</v>
@@ -4928,7 +4935,7 @@
         <v>141</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>80</v>
@@ -4949,7 +4956,7 @@
         <v>21</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>21</v>
@@ -4966,10 +4973,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>145</v>
@@ -5000,7 +5007,7 @@
         <v>147</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -5051,7 +5058,7 @@
         <v>21</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>80</v>
@@ -5089,10 +5096,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -5115,16 +5122,16 @@
         <v>93</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
@@ -5174,7 +5181,7 @@
         <v>21</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>80</v>
@@ -5183,7 +5190,7 @@
         <v>92</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>104</v>
@@ -5212,10 +5219,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -5241,13 +5248,13 @@
         <v>106</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
@@ -5273,13 +5280,13 @@
         <v>21</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="Z27" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="AA27" t="s" s="2">
         <v>21</v>
@@ -5297,7 +5304,7 @@
         <v>21</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>80</v>
@@ -5335,10 +5342,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5361,16 +5368,16 @@
         <v>93</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -5420,7 +5427,7 @@
         <v>21</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>80</v>
@@ -5441,7 +5448,7 @@
         <v>21</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>21</v>
@@ -5458,10 +5465,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5484,16 +5491,16 @@
         <v>93</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -5543,7 +5550,7 @@
         <v>21</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>80</v>
@@ -5581,10 +5588,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5607,16 +5614,16 @@
         <v>21</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5666,7 +5673,7 @@
         <v>21</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>80</v>
@@ -5681,13 +5688,13 @@
         <v>104</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>21</v>
@@ -5704,10 +5711,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5730,16 +5737,16 @@
         <v>93</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -5789,7 +5796,7 @@
         <v>21</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>80</v>
@@ -5807,10 +5814,10 @@
         <v>21</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>21</v>
@@ -5822,15 +5829,15 @@
         <v>21</v>
       </c>
       <c r="AQ31" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5853,13 +5860,13 @@
         <v>21</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5910,7 +5917,7 @@
         <v>21</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>80</v>
@@ -5931,7 +5938,7 @@
         <v>21</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>21</v>
@@ -5948,14 +5955,14 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
@@ -5977,13 +5984,13 @@
         <v>137</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -6033,7 +6040,7 @@
         <v>21</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>80</v>
@@ -6054,7 +6061,7 @@
         <v>21</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>21</v>
@@ -6071,14 +6078,14 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
@@ -6100,16 +6107,16 @@
         <v>137</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>21</v>
@@ -6158,7 +6165,7 @@
         <v>21</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>80</v>
@@ -6196,10 +6203,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -6225,13 +6232,13 @@
         <v>112</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -6257,13 +6264,13 @@
         <v>21</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>21</v>
@@ -6281,7 +6288,7 @@
         <v>21</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>92</v>
@@ -6299,10 +6306,10 @@
         <v>21</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>21</v>
@@ -6314,15 +6321,15 @@
         <v>21</v>
       </c>
       <c r="AQ35" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6345,13 +6352,13 @@
         <v>93</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6402,7 +6409,7 @@
         <v>21</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>92</v>
@@ -6420,10 +6427,10 @@
         <v>21</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>21</v>
@@ -6435,15 +6442,15 @@
         <v>21</v>
       </c>
       <c r="AQ36" t="s" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6466,19 +6473,19 @@
         <v>93</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>21</v>
@@ -6527,7 +6534,7 @@
         <v>21</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>80</v>
@@ -6548,7 +6555,7 @@
         <v>21</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>21</v>
@@ -6557,18 +6564,18 @@
         <v>21</v>
       </c>
       <c r="AP37" t="s" s="2">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="AQ37" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6591,19 +6598,19 @@
         <v>93</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>21</v>
@@ -6628,13 +6635,13 @@
         <v>21</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>21</v>
@@ -6652,7 +6659,7 @@
         <v>21</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>80</v>
@@ -6670,30 +6677,30 @@
         <v>21</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AP38" t="s" s="2">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="AQ38" t="s" s="2">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6716,13 +6723,13 @@
         <v>93</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6773,7 +6780,7 @@
         <v>21</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>92</v>
@@ -6791,10 +6798,10 @@
         <v>21</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>21</v>
@@ -6811,10 +6818,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6837,13 +6844,13 @@
         <v>21</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6894,7 +6901,7 @@
         <v>21</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>80</v>
@@ -6915,7 +6922,7 @@
         <v>21</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>21</v>
@@ -6932,14 +6939,14 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -6961,13 +6968,13 @@
         <v>137</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -7017,7 +7024,7 @@
         <v>21</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>80</v>
@@ -7038,7 +7045,7 @@
         <v>21</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>21</v>
@@ -7055,14 +7062,14 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
@@ -7084,16 +7091,16 @@
         <v>137</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>21</v>
@@ -7142,7 +7149,7 @@
         <v>21</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>80</v>
@@ -7180,10 +7187,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -7206,16 +7213,16 @@
         <v>93</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -7265,7 +7272,7 @@
         <v>21</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>92</v>
@@ -7277,36 +7284,36 @@
         <v>21</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AP43" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AQ43" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7329,13 +7336,13 @@
         <v>21</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -7386,7 +7393,7 @@
         <v>21</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>80</v>
@@ -7407,7 +7414,7 @@
         <v>21</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>21</v>
@@ -7424,14 +7431,14 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
@@ -7453,13 +7460,13 @@
         <v>137</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -7500,7 +7507,7 @@
         <v>140</v>
       </c>
       <c r="AC45" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AD45" t="s" s="2">
         <v>21</v>
@@ -7509,7 +7516,7 @@
         <v>141</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>80</v>
@@ -7530,7 +7537,7 @@
         <v>21</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>21</v>
@@ -7547,10 +7554,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7576,14 +7583,14 @@
         <v>112</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="P46" t="s" s="2">
         <v>21</v>
@@ -7596,7 +7603,7 @@
         <v>21</v>
       </c>
       <c r="T46" t="s" s="2">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="U46" t="s" s="2">
         <v>21</v>
@@ -7608,13 +7615,13 @@
         <v>21</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="Z46" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>21</v>
@@ -7632,7 +7639,7 @@
         <v>21</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>80</v>
@@ -7653,7 +7660,7 @@
         <v>21</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>21</v>
@@ -7662,7 +7669,7 @@
         <v>21</v>
       </c>
       <c r="AP46" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="AQ46" t="s" s="2">
         <v>21</v>
@@ -7670,10 +7677,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7699,14 +7706,14 @@
         <v>112</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="P47" t="s" s="2">
         <v>21</v>
@@ -7719,7 +7726,7 @@
         <v>21</v>
       </c>
       <c r="T47" t="s" s="2">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="U47" t="s" s="2">
         <v>21</v>
@@ -7755,7 +7762,7 @@
         <v>21</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>80</v>
@@ -7776,7 +7783,7 @@
         <v>21</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>21</v>
@@ -7793,10 +7800,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7819,19 +7826,19 @@
         <v>21</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="O48" t="s" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>21</v>
@@ -7880,7 +7887,7 @@
         <v>21</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>80</v>
@@ -7889,7 +7896,7 @@
         <v>92</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>104</v>
@@ -7901,7 +7908,7 @@
         <v>21</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>21</v>
@@ -7910,7 +7917,7 @@
         <v>21</v>
       </c>
       <c r="AP48" t="s" s="2">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="AQ48" t="s" s="2">
         <v>21</v>
@@ -7918,10 +7925,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7944,19 +7951,19 @@
         <v>93</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="O49" t="s" s="2">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>21</v>
@@ -7969,7 +7976,7 @@
         <v>21</v>
       </c>
       <c r="T49" t="s" s="2">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="U49" t="s" s="2">
         <v>21</v>
@@ -8005,7 +8012,7 @@
         <v>21</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>80</v>
@@ -8014,7 +8021,7 @@
         <v>92</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>104</v>
@@ -8026,7 +8033,7 @@
         <v>21</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>21</v>
@@ -8035,7 +8042,7 @@
         <v>21</v>
       </c>
       <c r="AP49" t="s" s="2">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="AQ49" t="s" s="2">
         <v>21</v>
@@ -8043,10 +8050,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -8069,19 +8076,19 @@
         <v>93</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="O50" t="s" s="2">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>21</v>
@@ -8130,7 +8137,7 @@
         <v>21</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>80</v>
@@ -8151,7 +8158,7 @@
         <v>21</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>21</v>
@@ -8168,10 +8175,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -8194,19 +8201,19 @@
         <v>93</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="O51" t="s" s="2">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>21</v>
@@ -8255,7 +8262,7 @@
         <v>21</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>80</v>
@@ -8276,7 +8283,7 @@
         <v>21</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>21</v>
@@ -8293,10 +8300,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8319,17 +8326,17 @@
         <v>93</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>21</v>
@@ -8342,7 +8349,7 @@
         <v>21</v>
       </c>
       <c r="T52" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="U52" t="s" s="2">
         <v>21</v>
@@ -8378,7 +8385,7 @@
         <v>21</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>80</v>
@@ -8399,7 +8406,7 @@
         <v>21</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>21</v>
@@ -8416,10 +8423,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8442,17 +8449,17 @@
         <v>93</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="P53" t="s" s="2">
         <v>21</v>
@@ -8501,7 +8508,7 @@
         <v>21</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>80</v>
@@ -8522,7 +8529,7 @@
         <v>21</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>21</v>
@@ -8539,10 +8546,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8565,16 +8572,16 @@
         <v>93</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -8600,11 +8607,11 @@
         <v>21</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Y54" s="2"/>
       <c r="Z54" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="AA54" t="s" s="2">
         <v>21</v>
@@ -8622,7 +8629,7 @@
         <v>21</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>80</v>
@@ -8640,13 +8647,13 @@
         <v>21</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="AO54" t="s" s="2">
         <v>21</v>
@@ -8655,15 +8662,15 @@
         <v>21</v>
       </c>
       <c r="AQ54" t="s" s="2">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8686,16 +8693,16 @@
         <v>93</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
@@ -8745,7 +8752,7 @@
         <v>21</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>80</v>
@@ -8766,7 +8773,7 @@
         <v>21</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>21</v>
@@ -8783,10 +8790,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8809,13 +8816,13 @@
         <v>21</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -8866,7 +8873,7 @@
         <v>21</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>80</v>
@@ -8887,7 +8894,7 @@
         <v>21</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>21</v>
@@ -8904,14 +8911,14 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
@@ -8933,13 +8940,13 @@
         <v>137</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
@@ -8989,7 +8996,7 @@
         <v>21</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>80</v>
@@ -9010,7 +9017,7 @@
         <v>21</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>21</v>
@@ -9027,14 +9034,14 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
@@ -9056,16 +9063,16 @@
         <v>137</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="O58" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="P58" t="s" s="2">
         <v>21</v>
@@ -9114,7 +9121,7 @@
         <v>21</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>80</v>
@@ -9152,10 +9159,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -9178,13 +9185,13 @@
         <v>21</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -9235,7 +9242,7 @@
         <v>21</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>80</v>
@@ -9250,19 +9257,19 @@
         <v>104</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>21</v>
       </c>
       <c r="AO59" t="s" s="2">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="AP59" t="s" s="2">
         <v>21</v>
@@ -9273,10 +9280,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -9299,16 +9306,16 @@
         <v>21</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -9334,13 +9341,13 @@
         <v>21</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="Z60" t="s" s="2">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="AA60" t="s" s="2">
         <v>21</v>
@@ -9358,7 +9365,7 @@
         <v>21</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>80</v>
@@ -9376,10 +9383,10 @@
         <v>21</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>21</v>
@@ -9391,15 +9398,15 @@
         <v>21</v>
       </c>
       <c r="AQ60" t="s" s="2">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9422,13 +9429,13 @@
         <v>93</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -9479,7 +9486,7 @@
         <v>21</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>80</v>
@@ -9497,13 +9504,13 @@
         <v>21</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="AO61" t="s" s="2">
         <v>21</v>
@@ -9512,15 +9519,15 @@
         <v>21</v>
       </c>
       <c r="AQ61" t="s" s="2">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9543,13 +9550,13 @@
         <v>21</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -9576,13 +9583,13 @@
         <v>21</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="Z62" t="s" s="2">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="AA62" t="s" s="2">
         <v>21</v>
@@ -9600,7 +9607,7 @@
         <v>21</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>80</v>
@@ -9618,13 +9625,13 @@
         <v>21</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="AO62" t="s" s="2">
         <v>21</v>
@@ -9633,15 +9640,15 @@
         <v>21</v>
       </c>
       <c r="AQ62" t="s" s="2">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9664,19 +9671,19 @@
         <v>21</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="O63" t="s" s="2">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="P63" t="s" s="2">
         <v>21</v>
@@ -9701,13 +9708,13 @@
         <v>21</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="Z63" t="s" s="2">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="AA63" t="s" s="2">
         <v>21</v>
@@ -9725,7 +9732,7 @@
         <v>21</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>80</v>
@@ -9743,13 +9750,13 @@
         <v>21</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="AO63" t="s" s="2">
         <v>21</v>
@@ -9758,15 +9765,15 @@
         <v>21</v>
       </c>
       <c r="AQ63" t="s" s="2">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9789,13 +9796,13 @@
         <v>21</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -9846,7 +9853,7 @@
         <v>21</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>80</v>
@@ -9864,13 +9871,13 @@
         <v>21</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AO64" t="s" s="2">
         <v>21</v>
@@ -9879,15 +9886,15 @@
         <v>21</v>
       </c>
       <c r="AQ64" t="s" s="2">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9910,16 +9917,16 @@
         <v>21</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
@@ -9969,7 +9976,7 @@
         <v>21</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>80</v>
@@ -9987,13 +9994,13 @@
         <v>21</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="AO65" t="s" s="2">
         <v>21</v>
@@ -10002,7 +10009,7 @@
         <v>21</v>
       </c>
       <c r="AQ65" t="s" s="2">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@e34e3e8fba242d44106420bca80860e4b36846f4 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-adi-documentreference.xlsx
+++ b/StructureDefinition-us-core-adi-documentreference.xlsx
@@ -3047,7 +3047,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" hidden="true">
+    <row r="10">
       <c r="A10" t="s" s="2">
         <v>145</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
         <v>171</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" hidden="true">
+    <row r="14">
       <c r="A14" t="s" s="2">
         <v>177</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
         <v>197</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" hidden="true">
+    <row r="18">
       <c r="A18" t="s" s="2">
         <v>225</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" hidden="true">
+    <row r="19">
       <c r="A19" t="s" s="2">
         <v>230</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
         <v>241</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" hidden="true">
+    <row r="21">
       <c r="A21" t="s" s="2">
         <v>251</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="32" hidden="true">
+    <row r="32">
       <c r="A32" t="s" s="2">
         <v>339</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" hidden="true">
+    <row r="36">
       <c r="A36" t="s" s="2">
         <v>347</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" hidden="true">
+    <row r="39">
       <c r="A39" t="s" s="2">
         <v>360</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" hidden="true">
+    <row r="41">
       <c r="A41" t="s" s="2">
         <v>377</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" hidden="true">
+    <row r="42">
       <c r="A42" t="s" s="2">
         <v>387</v>
       </c>
@@ -7602,7 +7602,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" hidden="true">
+    <row r="47">
       <c r="A47" t="s" s="2">
         <v>425</v>
       </c>
@@ -9072,12 +9072,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AQ58">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>